<commit_message>
Add training 5 material
</commit_message>
<xml_diff>
--- a/data/comparison.xlsx
+++ b/data/comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Desktop\desktop\R\Book\mpsi-data-training\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EC4339-1243-42E6-A23B-01CAD049D1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695E3A45-28D3-4119-9DD0-8FC5FC5E567E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{09C4DCFF-B5B4-4579-9423-97F222AE2FFC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09C4DCFF-B5B4-4579-9423-97F222AE2FFC}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="3" r:id="rId1"/>
@@ -228,13 +228,6 @@
 Datasets should be discoverable and citable (ex: metadata and DOI).</t>
   </si>
   <si>
-    <t>Examples include:
-Methodology and procedures used to collect the data
-Data labels
-Definitions of variables
-Any other information necessary to reproduce and understand the data</t>
-  </si>
-  <si>
     <t>Do you have any data covered by FERPA/HIPAA that doesn't allow data sharing?
 Do you work with any partners that do not allow you to share data (ex: School districts, Tribal regulations)?
 Are you working with proprietary data?</t>
@@ -266,6 +259,10 @@
   </si>
   <si>
     <t>Describe informed consent as well as how you will protect privacy and confidentiality "consistent with applicable federal, Tribal, state, and local laws, regulations, and policies"</t>
+  </si>
+  <si>
+    <t>Examples include:
+Methodology and procedures used to collect the data, Data labels, Definitions of variables, Any other information necessary to reproduce and understand the data</t>
   </si>
 </sst>
 </file>
@@ -842,16 +839,16 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="30.7265625" customWidth="1"/>
+    <col min="1" max="5" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -868,7 +865,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -885,7 +882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="173.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="173.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>35</v>
       </c>
@@ -896,7 +893,7 @@
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -913,7 +910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="351.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="351.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>36</v>
       </c>
@@ -930,7 +927,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -947,7 +944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="164.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>37</v>
       </c>
@@ -962,7 +959,7 @@
       </c>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
@@ -979,7 +976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="290" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="315" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -987,14 +984,14 @@
         <v>49</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>4</v>
       </c>
@@ -1011,7 +1008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>29</v>
       </c>
@@ -1026,7 +1023,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>5</v>
       </c>
@@ -1043,7 +1040,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="326.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="326.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>48</v>
       </c>
@@ -1060,7 +1057,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
@@ -1077,47 +1074,47 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="165" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="1" customFormat="1" ht="374.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" ht="374.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>18</v>
@@ -1126,9 +1123,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>12</v>
@@ -1143,15 +1140,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" ht="374.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" s="1" customFormat="1" ht="374.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>18</v>
@@ -1160,7 +1157,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>7</v>
       </c>
@@ -1177,7 +1174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" ht="289.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" s="1" customFormat="1" ht="289.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>9</v>
       </c>
@@ -1194,7 +1191,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>8</v>
       </c>
@@ -1211,7 +1208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="1" customFormat="1" ht="216" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" s="1" customFormat="1" ht="216" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>10</v>
       </c>
@@ -1236,23 +1233,23 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6328125" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1"/>
-    <col min="8" max="8" width="18.7265625" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="14.6328125" customWidth="1"/>
-    <col min="12" max="12" width="17.1796875" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1275,10 +1272,10 @@
         <v>6</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>7</v>
@@ -1287,7 +1284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1295,20 +1292,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>

</xml_diff>